<commit_message>
integrated midi-job function call into tb; more ssc tests
Former-commit-id: fe4c5bfb1dcde29aad58f751e764a2e5e57b313f
Former-commit-id: 474c10c7e93b42567c18f841951cd679ffee4e5d
</commit_message>
<xml_diff>
--- a/tests/test_tax_transfers/test_data/test_dfs_ssc.xlsx
+++ b/tests/test_tax_transfers/test_data/test_dfs_ssc.xlsx
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,7 @@
         <v>2018</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M13" si="1">S3+T3+U3+V3</f>
+        <f t="shared" ref="M3:M15" si="1">S3+T3+U3+V3</f>
         <v>96.153749999999988</v>
       </c>
       <c r="R3">
@@ -1235,10 +1235,126 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>111</v>
+      </c>
+      <c r="D14">
+        <v>700</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>2002</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>144.55000000000001</v>
+      </c>
+      <c r="R14">
+        <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(D14-400))</f>
+        <v>675.84999999999991</v>
+      </c>
+      <c r="S14" s="3">
+        <f>0.0955 *$D14</f>
+        <v>66.849999999999994</v>
+      </c>
+      <c r="T14" s="3">
+        <f>(0.0085 + (0.0025*(H14=TRUE)*(F14&gt;=23))) *D14</f>
+        <v>5.95</v>
+      </c>
+      <c r="U14" s="3">
+        <f>0.07 *$D14</f>
+        <v>49.000000000000007</v>
+      </c>
+      <c r="V14" s="3">
+        <f>0.0325 *$D14</f>
+        <v>22.75</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>4684</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2500</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>2019</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>433.37437499999999</v>
+      </c>
+      <c r="R15">
+        <f>0.7585*400+(((800/(800-400))-(400/(800-400)*0.7585))*(D15-400))</f>
+        <v>-193.20000000000005</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
+        <f>2*0.01525*MIN(I15,0.75*3115)</f>
+        <v>71.255624999999995</v>
+      </c>
+      <c r="U15" s="3">
+        <f>(0.073 + 0.082)*MIN(I15,0.75*3115)</f>
+        <v>362.11874999999998</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M16" s="2"/>

</xml_diff>